<commit_message>
BOM edits with substitutes
</commit_message>
<xml_diff>
--- a/Wally_BMS/Project Outputs for Wally_BMS/Wally_BMS_BOM.xlsx
+++ b/Wally_BMS/Project Outputs for Wally_BMS/Wally_BMS_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek Cao\Documents\wally-wally-wally\Hardware\Wally_BMS\Project Outputs for Wally_BMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061FA0ED-BEA4-410D-ADF1-3F02C64E6843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C634AAA3-E294-4A11-AAC6-F1E207ACF75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{047A0BC5-DE69-497F-A838-066B853D50ED}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="175">
   <si>
     <t>Description</t>
   </si>
@@ -114,15 +114,9 @@
     <t>DFE322520FD-1R0M=P2</t>
   </si>
   <si>
-    <t>MOSFET P-CH 30V 2A SOT23</t>
-  </si>
-  <si>
     <t>Q1, Q2, Q3, Q4</t>
   </si>
   <si>
-    <t>BSS308PEH6327XTSA1CT-ND</t>
-  </si>
-  <si>
     <t>Q10</t>
   </si>
   <si>
@@ -132,9 +126,6 @@
     <t>DMG2302UKQ-7</t>
   </si>
   <si>
-    <t>P20086CT-ND</t>
-  </si>
-  <si>
     <t>R23, R26, R29, R32</t>
   </si>
   <si>
@@ -348,12 +339,6 @@
     <t>FIXED IND 1UH 4.1A 22 MOHM SMD</t>
   </si>
   <si>
-    <t>BSS308PEH6327XTSA1</t>
-  </si>
-  <si>
-    <t>Infineon Technologies</t>
-  </si>
-  <si>
     <t>MOSFET N-CH 20V 2.8A SOT23 T&amp;R 3</t>
   </si>
   <si>
@@ -402,12 +387,6 @@
     <t>R12</t>
   </si>
   <si>
-    <t>R21, R24, R27, R30</t>
-  </si>
-  <si>
-    <t>R22, R25, R28, R31</t>
-  </si>
-  <si>
     <t>R33-R40</t>
   </si>
   <si>
@@ -483,12 +462,6 @@
     <t>RES 5.23K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t>ERJ-PB3B1002V</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 0.1% 1/5W 0603</t>
-  </si>
-  <si>
     <t>R8, R10</t>
   </si>
   <si>
@@ -510,18 +483,6 @@
     <t>RMCF0603FT20K0</t>
   </si>
   <si>
-    <t>541-1905-1-ND</t>
-  </si>
-  <si>
-    <t>PNM0402E5000BST1</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
-    <t>RES SMD 500 OHM 0.1% 1/20W 0402</t>
-  </si>
-  <si>
     <t>RMCF0402FT1K00CT-ND</t>
   </si>
   <si>
@@ -577,6 +538,30 @@
   </si>
   <si>
     <t>RES SMD 1K OHM 1% 1/4W 0603</t>
+  </si>
+  <si>
+    <t>MOSFET P-CH 30V 3A SOT23-3L</t>
+  </si>
+  <si>
+    <t>Alpha &amp; Omega Semiconductor Inc.</t>
+  </si>
+  <si>
+    <t>785-1459-1-ND</t>
+  </si>
+  <si>
+    <t>AO3421E</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD10K0CT-ND</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD10K0</t>
+  </si>
+  <si>
+    <t>RES 10K OHM 1% 1/8W 0603</t>
+  </si>
+  <si>
+    <t>R21, R22, R24, R25, R27, R28, R30, R31</t>
   </si>
 </sst>
 </file>
@@ -962,10 +947,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,99 +967,99 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4">
         <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4">
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4">
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1091,15 +1076,15 @@
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
@@ -1111,75 +1096,75 @@
         <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" s="4">
         <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C9" s="4">
         <v>12</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="F10" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="C10" s="4">
-        <v>2</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
@@ -1188,18 +1173,18 @@
         <v>2</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>9</v>
@@ -1214,12 +1199,12 @@
         <v>11</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>12</v>
@@ -1228,18 +1213,18 @@
         <v>2</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>14</v>
@@ -1248,13 +1233,13 @@
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E14" s="4">
         <v>3568</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1274,32 +1259,32 @@
         <v>18</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C16" s="4">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>19</v>
@@ -1314,12 +1299,12 @@
         <v>26013115</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>21</v>
@@ -1328,18 +1313,18 @@
         <v>2</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>22</v>
@@ -1354,407 +1339,387 @@
         <v>24</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="C20" s="4">
         <v>6</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>27</v>
+        <v>169</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>103</v>
+        <v>170</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>104</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="4">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="4">
-        <v>2</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F21" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C22" s="4">
         <v>2</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="F22" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="4">
-        <v>2</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="E23" s="4" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C24" s="4">
         <v>2</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C25" s="4">
         <v>5</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C26" s="4">
         <v>2</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C27" s="4">
         <v>2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>149</v>
+        <v>173</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C28" s="4">
         <v>12</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>31</v>
+        <v>171</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>148</v>
+        <v>172</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C29" s="4">
         <v>4</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" s="4">
+        <v>2</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C30" s="4">
-        <v>2</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>121</v>
+        <v>174</v>
       </c>
       <c r="C31" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>159</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>122</v>
+        <v>29</v>
       </c>
       <c r="C32" s="4">
         <v>6</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>161</v>
+        <v>30</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="C33" s="4">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>33</v>
+        <v>154</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C34" s="4">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>169</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C35" s="4">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C36" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>169</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>179</v>
+        <v>102</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>126</v>
+        <v>31</v>
       </c>
       <c r="C37" s="4">
-        <v>2</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>177</v>
+        <v>6</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>178</v>
+        <v>103</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="4">
+        <v>12</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="4">
-        <v>6</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="4">
-        <v>12</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed layout based on BOM updates
</commit_message>
<xml_diff>
--- a/Wally_BMS/Project Outputs for Wally_BMS/Wally_BMS_BOM.xlsx
+++ b/Wally_BMS/Project Outputs for Wally_BMS/Wally_BMS_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek Cao\Documents\wally-wally-wally\Hardware\Wally_BMS\Project Outputs for Wally_BMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72B6184-34B3-4EE0-AC78-9D5EA2A6615F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F3F7B-126F-4E7D-BB07-FC60A5FAFC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{047A0BC5-DE69-497F-A838-066B853D50ED}"/>
+    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{047A0BC5-DE69-497F-A838-066B853D50ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Wally_BMS" sheetId="1" r:id="rId1"/>
@@ -561,9 +561,6 @@
     <t>RES 10K OHM 1% 1/8W 0603</t>
   </si>
   <si>
-    <t>R21, R22, R24, R25, R27, R28, R30, R31</t>
-  </si>
-  <si>
     <t>CONN RCPT HSG 4POS 4.20MM</t>
   </si>
   <si>
@@ -571,6 +568,9 @@
   </si>
   <si>
     <t>WM22141-ND</t>
+  </si>
+  <si>
+    <t>R21, R22, R24, R25, R27, R28, R30, R31, R54-R57</t>
   </si>
 </sst>
 </file>
@@ -958,8 +958,8 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,15 +1551,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>150</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C30" s="4">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>148</v>
@@ -1733,16 +1733,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="C39" s="4">
         <v>3</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E39" s="4">
         <v>1727080004</v>

</xml_diff>

<commit_message>
removed thermistor, adjusted bga footprint to have more spacing
</commit_message>
<xml_diff>
--- a/Wally_BMS/Project Outputs for Wally_BMS/Wally_BMS_BOM.xlsx
+++ b/Wally_BMS/Project Outputs for Wally_BMS/Wally_BMS_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek Cao\Documents\wally-wally-wally\Hardware\Wally_BMS\Project Outputs for Wally_BMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F3F7B-126F-4E7D-BB07-FC60A5FAFC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD936368-0E67-4F8C-95AB-B3315993E4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{047A0BC5-DE69-497F-A838-066B853D50ED}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="181">
   <si>
     <t>Description</t>
   </si>
@@ -571,6 +571,15 @@
   </si>
   <si>
     <t>R21, R22, R24, R25, R27, R28, R30, R31, R54-R57</t>
+  </si>
+  <si>
+    <t>900-1727181111CT-ND</t>
+  </si>
+  <si>
+    <t>J2_2</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 16AWG CRIMP TIN</t>
   </si>
 </sst>
 </file>
@@ -958,8 +967,8 @@
   </sheetPr>
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,12 +1761,24 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
+      <c r="A40" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C40" s="4">
+        <v>10</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" s="4">
+        <v>1727181111</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>

</xml_diff>